<commit_message>
rename sheet1 to 2004-2013
</commit_message>
<xml_diff>
--- a/LifeExpectancy (Exercise 1).xlsx
+++ b/LifeExpectancy (Exercise 1).xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="၂၀၀၄-၂၀၁၃" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -98,12 +98,12 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,164 +399,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2004</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>62.1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>65.5</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>63.9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2005</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>62.3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>65.7</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>64.099999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>2006</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>62.7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>66.3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>64.599999999999994</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>2007</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>63.6</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>68</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>65.900000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>2008</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>64.2</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>68.3</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>66.2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>2009</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>64.5</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>68.400000000000006</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>66.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>2010</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>64.599999999999994</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>68.599999999999994</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>66.599999999999994</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>2011</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>64.900000000000006</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>68.7</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>67.3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>2012</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>65.099999999999994</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>68.900000000000006</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>67.400000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.85">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>2013</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>65.5</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>69.099999999999994</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>67.8</v>
       </c>
     </row>

</xml_diff>